<commit_message>
ci: bump nerdyscout/kicad-exports from v2.0 to v2.1 (#21)
* ci: bump nerdyscout/kicad-exports from v2.0 to v2.1

Bumps [nerdyscout/kicad-exports](https://github.com/nerdyscout/kicad-exports) from v2.0 to v2.1.
- [Release notes](https://github.com/nerdyscout/kicad-exports/releases)
- [Changelog](https://github.com/nerdyscout/kicad-exports/blob/master/CHANGELOG.md)
- [Commits](https://github.com/nerdyscout/kicad-exports/compare/v2.0...60350fc060ef3057fe6a3565357c6a9a8952f9cf)

Signed-off-by: dependabot[bot] <support@github.com>

* Fix pcbdraw path

"/opt/pcbdraw/pcbdraw" -> "/opt/pcbdraw"

* Add config files

Co-authored-by: dependabot[bot] <49699333+dependabot[bot]@users.noreply.github.com>
Co-authored-by: João Antônio Cardoso <joao.maker@gmail.com> 433d43cd027e91bda7b591c2774d215c25f60651
</commit_message>
<xml_diff>
--- a/hardware/bom/MCB19-bom.xlsx
+++ b/hardware/bom/MCB19-bom.xlsx
@@ -682,7 +682,7 @@
     <t>46</t>
   </si>
   <si>
-    <t>High-Speed CAN Transceiver, 1Mbps, 5V supply, SPLIT pin, -40C to +125C, SOIC8 package</t>
+    <t>High-Speed CAN Transceiver, 1Mbps, 5V supply, SPLIT pin, -40C to +125C, SOIC-8</t>
   </si>
   <si>
     <t>MCP2561-E-SN</t>
@@ -742,7 +742,7 @@
     <t>BoM Date:</t>
   </si>
   <si>
-    <t>Wed Oct 21 20:15:32 2020</t>
+    <t>Fri Oct 23 23:00:29 2020</t>
   </si>
   <si>
     <t>Schematic Source:</t>
@@ -754,7 +754,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>Eeschema 5.1.5+dfsg1-2~bpo10+1</t>
+    <t>Eeschema 5.1.6+dfsg1-1~bpo10+1</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
ci: bump nerdyscout/kicad-exports from v2.1 to v2.2 (#22)
Bumps [nerdyscout/kicad-exports](https://github.com/nerdyscout/kicad-exports) from v2.1 to v2.2.
- [Release notes](https://github.com/nerdyscout/kicad-exports/releases)
- [Changelog](https://github.com/nerdyscout/kicad-exports/blob/master/CHANGELOG.md)
- [Commits](https://github.com/nerdyscout/kicad-exports/compare/v2.1...4c23c0b2fd2f25ed36da3b85af3394ac87bb9c3c)

Signed-off-by: dependabot[bot] <support@github.com>

Co-authored-by: dependabot[bot] <49699333+dependabot[bot]@users.noreply.github.com> c05335776960523d464aaf4ec2702b455aec2ed9
</commit_message>
<xml_diff>
--- a/hardware/bom/MCB19-bom.xlsx
+++ b/hardware/bom/MCB19-bom.xlsx
@@ -742,7 +742,7 @@
     <t>BoM Date:</t>
   </si>
   <si>
-    <t>Mon Nov 16 17:05:48 2020</t>
+    <t>Mon Nov 16 17:06:31 2020</t>
   </si>
   <si>
     <t>Schematic Source:</t>
@@ -754,7 +754,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>Eeschema 5.1.6+dfsg1-1~bpo10+1</t>
+    <t>Eeschema 5.1.7+dfsg1-1~bpo10+1</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
ci: bump actions/upload-artifact from v2.2.0 to v2.2.1 (#24)
Bumps [actions/upload-artifact](https://github.com/actions/upload-artifact) from v2.2.0 to v2.2.1.
- [Release notes](https://github.com/actions/upload-artifact/releases)
- [Commits](https://github.com/actions/upload-artifact/compare/v2.2.0...726a6dcd0199f578459862705eed35cda05af50b)

Signed-off-by: dependabot[bot] <support@github.com>

Co-authored-by: dependabot[bot] <49699333+dependabot[bot]@users.noreply.github.com> a1355769c907fcd18c5a51e30c1ef1eb28cc17e7
</commit_message>
<xml_diff>
--- a/hardware/bom/MCB19-bom.xlsx
+++ b/hardware/bom/MCB19-bom.xlsx
@@ -742,7 +742,7 @@
     <t>BoM Date:</t>
   </si>
   <si>
-    <t>Mon Nov 16 17:06:31 2020</t>
+    <t>Mon Nov 16 17:06:06 2020</t>
   </si>
   <si>
     <t>Schematic Source:</t>
@@ -754,7 +754,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>Eeschema 5.1.7+dfsg1-1~bpo10+1</t>
+    <t>Eeschema 5.1.6+dfsg1-1~bpo10+1</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
ci: bump actions/download-artifact from v2.0.6 to v2.0.7 (#25)
Bumps [actions/download-artifact](https://github.com/actions/download-artifact) from v2.0.6 to v2.0.7.
- [Release notes](https://github.com/actions/download-artifact/releases)
- [Commits](https://github.com/actions/download-artifact/compare/v2.0.6...f144d3c3916a86f4d6b11ff379d17a49d8f85dbc)

Signed-off-by: dependabot[bot] <support@github.com>

Co-authored-by: dependabot[bot] <49699333+dependabot[bot]@users.noreply.github.com> 7d982ee5fddb3a6e3f5694803fb4e0d471456e0f
</commit_message>
<xml_diff>
--- a/hardware/bom/MCB19-bom.xlsx
+++ b/hardware/bom/MCB19-bom.xlsx
@@ -742,7 +742,7 @@
     <t>BoM Date:</t>
   </si>
   <si>
-    <t>Mon Nov 16 17:06:06 2020</t>
+    <t>Wed Dec 16 15:11:17 2020</t>
   </si>
   <si>
     <t>Schematic Source:</t>
@@ -754,7 +754,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>Eeschema 5.1.6+dfsg1-1~bpo10+1</t>
+    <t>Eeschema 5.1.7+dfsg1-1~bpo10+1</t>
   </si>
 </sst>
 </file>

</xml_diff>